<commit_message>
Data Driven Test Scripting is done.
</commit_message>
<xml_diff>
--- a/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
+++ b/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\source\repos\OrangeHRM_Playwright_DotNet\OrangeHRM_Playwright_DotNet\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai.islam\source\repos\OrangeHRM_Playwright_DotNet\OrangeHRM_Playwright_DotNet\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C7C253-E4DF-40C7-AEA2-1787E3125656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E58263-02E3-480C-8234-BE8F1CE20769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginData" sheetId="1" r:id="rId1"/>
+    <sheet name="AddAdminData" sheetId="2" r:id="rId2"/>
+    <sheet name="SearchData" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,16 +27,79 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>EmployeeName</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>amelia</t>
+  </si>
+  <si>
+    <t>amelia123</t>
+  </si>
+  <si>
+    <t>Ravi M B</t>
+  </si>
+  <si>
+    <t>ravimb</t>
+  </si>
+  <si>
+    <t>ravimb123</t>
+  </si>
+  <si>
+    <t>James  Butler</t>
+  </si>
+  <si>
+    <t>james</t>
+  </si>
+  <si>
+    <t>james123</t>
+  </si>
+  <si>
+    <t>Amelia  Brown</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>abcde123</t>
+  </si>
+  <si>
+    <t>abcde124</t>
+  </si>
+  <si>
+    <t>James Butler</t>
+  </si>
   <si>
     <t>Amelia Brown</t>
+  </si>
+  <si>
+    <t>FMLName</t>
+  </si>
+  <si>
+    <t>Qwerty Lname</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -42,16 +107,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -59,12 +136,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,9 +177,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -123,7 +217,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -229,7 +323,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -371,7 +465,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -379,20 +473,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DC939D-A7EE-4A7C-B2D3-D794362D006C}">
-  <dimension ref="B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6431BB-4EDA-4EE6-BDD0-BA2675F2E25D}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.36328125" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" customWidth="1"/>
+    <col min="3" max="3" width="10.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537DA4D0-0C77-407F-B79F-0ED3CFB8392D}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTML report is generated and Codes are updated.
</commit_message>
<xml_diff>
--- a/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
+++ b/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai.islam\source\repos\OrangeHRM_Playwright_DotNet\OrangeHRM_Playwright_DotNet\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\source\repos\OrangeHRM_Playwright_DotNet\OrangeHRM_Playwright_DotNet\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E58263-02E3-480C-8234-BE8F1CE20769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D34136D-F8FA-4832-AD4B-2368AD0E09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
+    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>UserName</t>
   </si>
@@ -68,9 +68,6 @@
     <t>james</t>
   </si>
   <si>
-    <t>james123</t>
-  </si>
-  <si>
     <t>Amelia  Brown</t>
   </si>
   <si>
@@ -83,9 +80,6 @@
     <t>abcde124</t>
   </si>
   <si>
-    <t>James Butler</t>
-  </si>
-  <si>
     <t>Amelia Brown</t>
   </si>
   <si>
@@ -93,6 +87,15 @@
   </si>
   <si>
     <t>Qwerty Lname</t>
+  </si>
+  <si>
+    <t>Mohai Islam</t>
+  </si>
+  <si>
+    <t>mohai123</t>
+  </si>
+  <si>
+    <t>mohai1</t>
   </si>
 </sst>
 </file>
@@ -177,9 +180,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -217,7 +220,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -323,7 +326,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -465,7 +468,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -475,7 +478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13DC939D-A7EE-4A7C-B2D3-D794362D006C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -503,10 +506,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -514,12 +517,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -539,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6431BB-4EDA-4EE6-BDD0-BA2675F2E25D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -581,21 +584,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>
@@ -636,10 +639,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -652,7 +655,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Code optimized and updated.
</commit_message>
<xml_diff>
--- a/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
+++ b/OrangeHRM_Playwright_DotNet/TestData/Data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohai\source\repos\OrangeHRM_Playwright_DotNet\OrangeHRM_Playwright_DotNet\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D34136D-F8FA-4832-AD4B-2368AD0E09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4EF378-4DD1-4134-9D2B-F7EB7BEAE9B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="14400" windowHeight="7270" activeTab="1" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{0CDDB4FA-CFE4-4651-96EB-0FD46E3F3D47}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
-    <sheet name="AddAdminData" sheetId="2" r:id="rId2"/>
-    <sheet name="SearchData" sheetId="3" r:id="rId3"/>
+    <sheet name="ChangePassword" sheetId="4" r:id="rId2"/>
+    <sheet name="AddAdminData" sheetId="2" r:id="rId3"/>
+    <sheet name="SearchData" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>UserName</t>
   </si>
@@ -96,13 +97,19 @@
   </si>
   <si>
     <t>mohai1</t>
+  </si>
+  <si>
+    <t>NewPassword</t>
+  </si>
+  <si>
+    <t>admin@123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +123,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,6 +142,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -155,15 +176,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -539,10 +564,49 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5366E7EB-016F-4A7E-8663-B4FFF96A318B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{0A65C128-D020-44F5-807A-52330EF05287}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{792EEF36-50F1-418B-9012-3A67B17F1A17}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F6431BB-4EDA-4EE6-BDD0-BA2675F2E25D}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -615,7 +679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{537DA4D0-0C77-407F-B79F-0ED3CFB8392D}">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>